<commit_message>
changes to zeitplan and added portal
</commit_message>
<xml_diff>
--- a/docs/Zeitplan.xlsx
+++ b/docs/Zeitplan.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24014"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{E14DC542-80DB-46BF-9A63-294E762A6250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -258,7 +257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -756,22 +755,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,24 +789,40 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Komma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
+    <cellStyle name="Name" xfId="11"/>
+    <cellStyle name="Project Start" xfId="9"/>
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Überschrift" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -951,7 +950,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="11"/>
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="totalRow" dxfId="9"/>
@@ -1315,7 +1314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1323,7 +1322,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS3" sqref="AS3"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1358,17 +1357,17 @@
       <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="71">
+      <c r="D2" s="70"/>
+      <c r="E2" s="68">
         <v>44293</v>
       </c>
-      <c r="F2" s="71"/>
+      <c r="F2" s="68"/>
       <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,117 +1375,117 @@
         <v>7</v>
       </c>
       <c r="B3" s="40"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="71">
+      <c r="D3" s="69"/>
+      <c r="E3" s="68">
         <v>44330</v>
       </c>
-      <c r="F3" s="71"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="56">
+      <c r="I4" s="65">
         <f>I5</f>
         <v>44291</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="56">
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="65">
         <f>P5</f>
         <v>44298</v>
       </c>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="56">
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="65">
         <f>W5</f>
         <v>44305</v>
       </c>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="56">
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="65">
         <f>AD5</f>
         <v>44312</v>
       </c>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="56">
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="65">
         <f>AK5</f>
         <v>44319</v>
       </c>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="57"/>
-      <c r="AO4" s="57"/>
-      <c r="AP4" s="57"/>
-      <c r="AQ4" s="58"/>
-      <c r="AR4" s="56">
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="67"/>
+      <c r="AR4" s="65">
         <f>AR5</f>
         <v>44326</v>
       </c>
-      <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
-      <c r="AV4" s="57"/>
-      <c r="AW4" s="57"/>
-      <c r="AX4" s="58"/>
-      <c r="AY4" s="56">
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="66"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="66"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="65">
         <f>AY5</f>
         <v>44333</v>
       </c>
-      <c r="AZ4" s="57"/>
-      <c r="BA4" s="57"/>
-      <c r="BB4" s="57"/>
-      <c r="BC4" s="57"/>
-      <c r="BD4" s="57"/>
-      <c r="BE4" s="58"/>
-      <c r="BF4" s="56">
+      <c r="AZ4" s="66"/>
+      <c r="BA4" s="66"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="66"/>
+      <c r="BD4" s="66"/>
+      <c r="BE4" s="67"/>
+      <c r="BF4" s="65">
         <f>BF5</f>
         <v>44340</v>
       </c>
-      <c r="BG4" s="57"/>
-      <c r="BH4" s="57"/>
-      <c r="BI4" s="57"/>
-      <c r="BJ4" s="57"/>
-      <c r="BK4" s="57"/>
-      <c r="BL4" s="58"/>
+      <c r="BG4" s="66"/>
+      <c r="BH4" s="66"/>
+      <c r="BI4" s="66"/>
+      <c r="BJ4" s="66"/>
+      <c r="BK4" s="66"/>
+      <c r="BL4" s="67"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44291</v>
@@ -2113,11 +2112,11 @@
       <c r="D9" s="21">
         <v>1</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="53">
         <f>Project_Start</f>
         <v>44293</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="53">
         <v>44311</v>
       </c>
       <c r="G9" s="16"/>
@@ -2195,10 +2194,10 @@
       <c r="D10" s="21">
         <v>1</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="53">
         <v>44294</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="53">
         <v>44294</v>
       </c>
       <c r="G10" s="16"/>
@@ -2274,10 +2273,10 @@
       <c r="D11" s="21">
         <v>1</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="53">
         <v>44294</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="53">
         <v>44312</v>
       </c>
       <c r="G11" s="16"/>
@@ -2353,10 +2352,10 @@
       <c r="D12" s="21">
         <v>1</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="53">
         <v>44294</v>
       </c>
-      <c r="F12" s="59">
+      <c r="F12" s="53">
         <v>44305</v>
       </c>
       <c r="G12" s="16"/>
@@ -2432,10 +2431,10 @@
       <c r="D13" s="21">
         <v>1</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="53">
         <v>44294</v>
       </c>
-      <c r="F13" s="59">
+      <c r="F13" s="53">
         <v>44301</v>
       </c>
       <c r="G13" s="16"/>
@@ -2509,8 +2508,8 @@
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="61"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="str">
         <f t="shared" si="6"/>
@@ -2584,10 +2583,10 @@
       <c r="D15" s="24">
         <v>1</v>
       </c>
-      <c r="E15" s="62">
+      <c r="E15" s="56">
         <v>44298</v>
       </c>
-      <c r="F15" s="62">
+      <c r="F15" s="56">
         <v>44301</v>
       </c>
       <c r="G15" s="16"/>
@@ -2663,10 +2662,10 @@
       <c r="D16" s="24">
         <v>1</v>
       </c>
-      <c r="E16" s="62">
+      <c r="E16" s="56">
         <v>44298</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="56">
         <f>E16+7</f>
         <v>44305</v>
       </c>
@@ -2740,10 +2739,10 @@
       <c r="D17" s="24">
         <v>1</v>
       </c>
-      <c r="E17" s="62">
+      <c r="E17" s="56">
         <v>44300</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="56">
         <v>44301</v>
       </c>
       <c r="G17" s="16"/>
@@ -2819,11 +2818,11 @@
       <c r="D18" s="24">
         <v>1</v>
       </c>
-      <c r="E18" s="62">
+      <c r="E18" s="56">
         <f>F17</f>
         <v>44301</v>
       </c>
-      <c r="F18" s="62">
+      <c r="F18" s="56">
         <f>E18+3</f>
         <v>44304</v>
       </c>
@@ -2900,10 +2899,10 @@
       <c r="D19" s="24">
         <v>1</v>
       </c>
-      <c r="E19" s="62">
+      <c r="E19" s="56">
         <v>44300</v>
       </c>
-      <c r="F19" s="62">
+      <c r="F19" s="56">
         <v>44307</v>
       </c>
       <c r="G19" s="16"/>
@@ -2976,10 +2975,10 @@
       <c r="D20" s="24">
         <v>1</v>
       </c>
-      <c r="E20" s="62">
+      <c r="E20" s="56">
         <v>44305</v>
       </c>
-      <c r="F20" s="62">
+      <c r="F20" s="56">
         <v>44310</v>
       </c>
       <c r="G20" s="16"/>
@@ -3053,8 +3052,8 @@
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="26"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16" t="str">
         <f t="shared" si="6"/>
@@ -3126,12 +3125,12 @@
         <v>33</v>
       </c>
       <c r="D22" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="E22" s="65">
+        <v>1</v>
+      </c>
+      <c r="E22" s="59">
         <v>44305</v>
       </c>
-      <c r="F22" s="65">
+      <c r="F22" s="59">
         <v>44326</v>
       </c>
       <c r="G22" s="16"/>
@@ -3205,12 +3204,12 @@
         <v>35</v>
       </c>
       <c r="D23" s="27">
-        <v>0.8</v>
-      </c>
-      <c r="E23" s="65">
+        <v>1</v>
+      </c>
+      <c r="E23" s="59">
         <v>44308</v>
       </c>
-      <c r="F23" s="65">
+      <c r="F23" s="59">
         <v>44316</v>
       </c>
       <c r="G23" s="16"/>
@@ -3284,12 +3283,12 @@
         <v>29</v>
       </c>
       <c r="D24" s="27">
-        <v>0</v>
-      </c>
-      <c r="E24" s="65">
+        <v>1</v>
+      </c>
+      <c r="E24" s="59">
         <v>44312</v>
       </c>
-      <c r="F24" s="65">
+      <c r="F24" s="59">
         <v>44316</v>
       </c>
       <c r="G24" s="16"/>
@@ -3360,12 +3359,12 @@
         <v>29</v>
       </c>
       <c r="D25" s="27">
-        <v>0</v>
-      </c>
-      <c r="E25" s="65">
+        <v>1</v>
+      </c>
+      <c r="E25" s="59">
         <v>44316</v>
       </c>
-      <c r="F25" s="65">
+      <c r="F25" s="59">
         <v>44319</v>
       </c>
       <c r="G25" s="16"/>
@@ -3439,12 +3438,12 @@
         <v>28</v>
       </c>
       <c r="D26" s="27">
-        <v>0</v>
-      </c>
-      <c r="E26" s="65">
+        <v>1</v>
+      </c>
+      <c r="E26" s="59">
         <v>44316</v>
       </c>
-      <c r="F26" s="65">
+      <c r="F26" s="59">
         <v>44322</v>
       </c>
       <c r="G26" s="16"/>
@@ -3511,19 +3510,19 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="64" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="E27" s="65">
+        <v>1</v>
+      </c>
+      <c r="E27" s="59">
         <v>44312</v>
       </c>
-      <c r="F27" s="65">
+      <c r="F27" s="59">
         <v>44326</v>
       </c>
       <c r="G27" s="16"/>
@@ -3597,8 +3596,8 @@
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="29"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="67"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="61"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16" t="str">
         <f t="shared" si="6"/>
@@ -3670,12 +3669,12 @@
         <v>33</v>
       </c>
       <c r="D29" s="30">
-        <v>0</v>
-      </c>
-      <c r="E29" s="68">
+        <v>1</v>
+      </c>
+      <c r="E29" s="62">
         <v>44319</v>
       </c>
-      <c r="F29" s="68">
+      <c r="F29" s="62">
         <v>44326</v>
       </c>
       <c r="G29" s="16"/>
@@ -3749,18 +3748,18 @@
         <v>41</v>
       </c>
       <c r="D30" s="30">
-        <v>0</v>
-      </c>
-      <c r="E30" s="68">
+        <v>1</v>
+      </c>
+      <c r="E30" s="62">
         <v>44325</v>
       </c>
-      <c r="F30" s="68">
-        <v>44330</v>
+      <c r="F30" s="62">
+        <v>44340</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="16">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
@@ -3828,12 +3827,12 @@
         <v>33</v>
       </c>
       <c r="D31" s="30">
-        <v>0</v>
-      </c>
-      <c r="E31" s="68">
+        <v>1</v>
+      </c>
+      <c r="E31" s="62">
         <v>44319</v>
       </c>
-      <c r="F31" s="68">
+      <c r="F31" s="62">
         <v>44323</v>
       </c>
       <c r="G31" s="16"/>
@@ -3907,18 +3906,18 @@
         <v>55</v>
       </c>
       <c r="D32" s="30">
-        <v>0</v>
-      </c>
-      <c r="E32" s="68">
+        <v>1</v>
+      </c>
+      <c r="E32" s="62">
         <v>44320</v>
       </c>
-      <c r="F32" s="68">
-        <v>44330</v>
+      <c r="F32" s="62">
+        <v>44340</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
@@ -3986,18 +3985,18 @@
         <v>19</v>
       </c>
       <c r="D33" s="30">
-        <v>0</v>
-      </c>
-      <c r="E33" s="68">
+        <v>1</v>
+      </c>
+      <c r="E33" s="62">
         <v>44319</v>
       </c>
-      <c r="F33" s="68">
-        <v>44330</v>
+      <c r="F33" s="62">
+        <v>44340</v>
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="16">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I33" s="31"/>
       <c r="J33" s="31"/>
@@ -4068,6 +4067,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E2:F2"/>
@@ -4076,12 +4081,6 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4111,7 +4110,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>